<commit_message>
modify hlb pattern and fix hlb filename bug
</commit_message>
<xml_diff>
--- a/data/ID映射表.xlsx
+++ b/data/ID映射表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="157">
   <si>
     <t>ID</t>
   </si>
@@ -246,6 +246,18 @@
     <t>韩朝阳</t>
   </si>
   <si>
+    <t>罗天宇</t>
+  </si>
+  <si>
+    <t>张瑞</t>
+  </si>
+  <si>
+    <t>张瑞1</t>
+  </si>
+  <si>
+    <t>刘明虎</t>
+  </si>
+  <si>
     <t>代理合计</t>
   </si>
   <si>
@@ -279,12 +291,6 @@
     <t>仝鹏辉</t>
   </si>
   <si>
-    <t>张瑞</t>
-  </si>
-  <si>
-    <t>张瑞1</t>
-  </si>
-  <si>
     <t>公司</t>
   </si>
   <si>
@@ -309,6 +315,9 @@
     <t>王川（卡商潢川店）</t>
   </si>
   <si>
+    <t>王德海;卡商潢川店</t>
+  </si>
+  <si>
     <t>杨勇12580;孙良友;涂银</t>
   </si>
   <si>
@@ -333,12 +342,18 @@
     <t>李登辉（河南融鼎科技有限公司）</t>
   </si>
   <si>
-    <t>河南融鼎科技有限公司</t>
+    <t>河南融鼎电子科技有限公司;荣鼎科技分公司</t>
+  </si>
+  <si>
+    <t>苏杰代理;灵创科技</t>
   </si>
   <si>
     <t>潘云飞</t>
   </si>
   <si>
+    <t>潘云飞;齐达伟</t>
+  </si>
+  <si>
     <t>李莎;丁富军</t>
   </si>
   <si>
@@ -357,12 +372,33 @@
     <t>任航行</t>
   </si>
   <si>
+    <t>陈鹏88;周姣</t>
+  </si>
+  <si>
     <t>唐晓辉（中盛普惠）</t>
   </si>
   <si>
     <t>中盛普惠</t>
   </si>
   <si>
+    <t>吴鹏（豫洗人家）</t>
+  </si>
+  <si>
+    <t>豫洗人家</t>
+  </si>
+  <si>
+    <t>胡伟</t>
+  </si>
+  <si>
+    <t>岑文燃</t>
+  </si>
+  <si>
+    <t>徐永华（王源）</t>
+  </si>
+  <si>
+    <t>徐永华</t>
+  </si>
+  <si>
     <t>张民坤88</t>
   </si>
   <si>
@@ -387,9 +423,21 @@
     <t>合利宝映射</t>
   </si>
   <si>
+    <t>岳双(信阳市聚成电子科技有限公司 )</t>
+  </si>
+  <si>
+    <t>信阳市聚成电子科技有限公司;闵伟;朱帅安;任铭;胡吉祥;高宇航;张从阳;朱海晶</t>
+  </si>
+  <si>
     <t>杨勇;付然;涂银银</t>
   </si>
   <si>
+    <t>高强;李伟</t>
+  </si>
+  <si>
+    <t>胡俊远;张涛</t>
+  </si>
+  <si>
     <t>丁哲</t>
   </si>
   <si>
@@ -399,19 +447,40 @@
     <t>罗瑞</t>
   </si>
   <si>
-    <t>岳双(信阳市聚成电子科技有限公司 )</t>
-  </si>
-  <si>
-    <t>信阳市聚成电子科技有限公司;闵伟;朱帅安;任铭</t>
-  </si>
-  <si>
     <t>张加豪</t>
   </si>
   <si>
+    <t>张加豪;李阳;李士峰</t>
+  </si>
+  <si>
+    <t>周小启;陶世亮</t>
+  </si>
+  <si>
     <t>赵俊辉</t>
   </si>
   <si>
     <t>蔡童茹</t>
+  </si>
+  <si>
+    <t>罗帅;孙建;宋兴冰</t>
+  </si>
+  <si>
+    <t>李登辉;张雪</t>
+  </si>
+  <si>
+    <t>梁明</t>
+  </si>
+  <si>
+    <t>陈保忠(陈健）</t>
+  </si>
+  <si>
+    <t>胡德红(付翔宇)</t>
+  </si>
+  <si>
+    <t>胡德红;付翔宇</t>
+  </si>
+  <si>
+    <t>李勇;徐亚龙</t>
   </si>
   <si>
     <t>张民坤;伍绍圣;何武峰</t>
@@ -426,17 +495,30 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -452,28 +534,58 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF333333"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
+      <color rgb="FF000000"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,7 +598,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -509,7 +621,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -522,30 +657,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -559,15 +673,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -582,30 +694,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -613,6 +701,96 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -622,25 +800,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,37 +824,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,109 +884,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -807,6 +895,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -825,50 +952,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -902,8 +990,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -915,10 +1003,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -927,34 +1015,37 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -963,145 +1054,169 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1434,15 +1549,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A63" sqref="$A63:$XFD63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A66" sqref="$A66:$XFD66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="22" customHeight="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="29.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1450,7 +1569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" customHeight="1" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1458,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" customHeight="1" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1466,7 +1585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1474,7 +1593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" customHeight="1" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1482,7 +1601,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" customHeight="1" spans="1:2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" customHeight="1" spans="1:2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1498,7 +1617,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" customHeight="1" spans="1:2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1506,7 +1625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" customHeight="1" spans="1:2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1514,7 +1633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" customHeight="1" spans="1:2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1522,7 +1641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" customHeight="1" spans="1:2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1530,7 +1649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" customHeight="1" spans="1:2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1538,7 +1657,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" customHeight="1" spans="1:2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1546,7 +1665,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" customHeight="1" spans="1:2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1554,7 +1673,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" customHeight="1" spans="1:2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1562,7 +1681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" customHeight="1" spans="1:2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1570,7 +1689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" customHeight="1" spans="1:2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1578,7 +1697,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" customHeight="1" spans="1:2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1586,7 +1705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" customHeight="1" spans="1:2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1594,7 +1713,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" customHeight="1" spans="1:2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1602,7 +1721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" customHeight="1" spans="1:2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1610,7 +1729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" customHeight="1" spans="1:2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1618,7 +1737,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" customHeight="1" spans="1:2">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1626,7 +1745,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" customHeight="1" spans="1:2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1634,7 +1753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" customHeight="1" spans="1:2">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1642,7 +1761,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" customHeight="1" spans="1:2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1650,7 +1769,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" customHeight="1" spans="1:2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1658,7 +1777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" customHeight="1" spans="1:2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1666,7 +1785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" customHeight="1" spans="1:2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1674,7 +1793,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" customHeight="1" spans="1:2">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1682,7 +1801,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" customHeight="1" spans="1:2">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1690,7 +1809,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" customHeight="1" spans="1:2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -1698,7 +1817,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" customHeight="1" spans="1:2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1706,7 +1825,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" customHeight="1" spans="1:2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1714,7 +1833,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" customHeight="1" spans="1:2">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1722,7 +1841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" customHeight="1" spans="1:2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1730,7 +1849,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" customHeight="1" spans="1:2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1738,7 +1857,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" customHeight="1" spans="1:2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -1746,7 +1865,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" customHeight="1" spans="1:2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -1754,7 +1873,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" customHeight="1" spans="1:2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -1762,7 +1881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" customHeight="1" spans="1:2">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1770,7 +1889,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" customHeight="1" spans="1:2">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1778,7 +1897,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" customHeight="1" spans="1:2">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1786,7 +1905,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" customHeight="1" spans="1:2">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1794,7 +1913,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" customHeight="1" spans="1:2">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -1802,7 +1921,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" customHeight="1" spans="1:2">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -1810,7 +1929,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" customHeight="1" spans="1:2">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -1818,7 +1937,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" customHeight="1" spans="1:2">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -1826,7 +1945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" customHeight="1" spans="1:2">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -1834,7 +1953,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" customHeight="1" spans="1:2">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -1842,7 +1961,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" customHeight="1" spans="1:2">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -1850,7 +1969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" customHeight="1" spans="1:2">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -1858,7 +1977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" customHeight="1" spans="1:2">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -1866,7 +1985,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" customHeight="1" spans="1:2">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -1874,7 +1993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" customHeight="1" spans="1:2">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -1882,7 +2001,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" customHeight="1" spans="1:2">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -1890,7 +2009,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" customHeight="1" spans="1:2">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -1898,7 +2017,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" customHeight="1" spans="1:2">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -1906,7 +2025,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" customHeight="1" spans="1:2">
       <c r="A59" t="s">
         <v>72</v>
       </c>
@@ -1914,7 +2033,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" customHeight="1" spans="1:2">
       <c r="A60" t="s">
         <v>73</v>
       </c>
@@ -1922,7 +2041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" customHeight="1" spans="1:2">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -1930,7 +2049,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" customHeight="1" spans="1:2">
       <c r="A62" t="s">
         <v>75</v>
       </c>
@@ -1938,7 +2057,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" customHeight="1" spans="1:2">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -1946,31 +2065,31 @@
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" customHeight="1" spans="1:2">
       <c r="A64" t="s">
         <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" customHeight="1" spans="1:2">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" customHeight="1" spans="1:2">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B66" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" customHeight="1" spans="1:2">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -1978,7 +2097,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" customHeight="1" spans="1:2">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -1986,7 +2105,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" customHeight="1" spans="1:2">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -1994,7 +2113,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" customHeight="1" spans="1:2">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -2002,7 +2121,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" customHeight="1" spans="1:2">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -2010,7 +2129,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" customHeight="1" spans="1:2">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -2018,12 +2137,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" customHeight="1" spans="1:2">
       <c r="A73" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="B73" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" customHeight="1" spans="1:2">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -2031,42 +2153,55 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" customHeight="1" spans="1:1">
       <c r="A75" t="s">
         <v>91</v>
       </c>
-      <c r="B75" t="s">
+    </row>
+    <row r="76" customHeight="1" spans="1:2">
+      <c r="A76" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
+      <c r="B76" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="77" customHeight="1" spans="1:2">
+      <c r="A77" t="s">
         <v>93</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="78" customHeight="1" spans="1:2">
+      <c r="A78" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B35">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B64">
+  <conditionalFormatting sqref="B67">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
+  <conditionalFormatting sqref="B71">
     <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A$1:A$1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A76">
+  <conditionalFormatting sqref="A1:A78">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B34 B36:B63 B65:B67 B69:B76">
+  <conditionalFormatting sqref="B1:B34 B36:B66 B68:B70 B72:B78">
     <cfRule type="duplicateValues" dxfId="0" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2078,282 +2213,390 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.05" customHeight="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="35.8833333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33.775" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="2" max="2" width="33.775" style="18" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="20.125" style="11" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:2">
+    <row r="1" ht="15" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:2">
+      <c r="B1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:2">
+        <v>98</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:2">
+      <c r="B3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:2">
-      <c r="A5" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" customHeight="1" spans="1:2">
+      <c r="B4" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" customHeight="1" spans="1:2">
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" customHeight="1" spans="1:2">
+        <v>105</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:2">
+        <v>85</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:2">
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:2">
+        <v>106</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" customHeight="1" spans="1:2">
-      <c r="A12" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:2">
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" ht="28.5" spans="1:4">
+      <c r="A12" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:2">
+      <c r="B13" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="15" customHeight="1" spans="1:2">
+        <v>110</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" customHeight="1" spans="1:2">
+      <c r="B15" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" customHeight="1" spans="1:2">
+        <v>113</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="22"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" customHeight="1" spans="1:2">
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" customHeight="1" spans="1:2">
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" customHeight="1" spans="1:2">
+        <v>114</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="1:2">
+        <v>115</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="21"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="21"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="21"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="21"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="23"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" customHeight="1" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" customHeight="1" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" customHeight="1" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" customHeight="1" spans="1:2">
-      <c r="A26" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" customHeight="1" spans="1:2">
-      <c r="A27" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" customHeight="1" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="B32" s="18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" customHeight="1" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" customHeight="1" spans="1:2">
-      <c r="A30" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" customHeight="1" spans="1:2">
-      <c r="A31" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" customHeight="1" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="33" customHeight="1" spans="1:2">
+      <c r="C32" s="13"/>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="E35" s="13"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="E37" s="13"/>
+    </row>
+    <row r="38" spans="3:5">
+      <c r="C38" s="13"/>
+      <c r="E38" s="13"/>
+    </row>
+    <row r="39" spans="3:5">
+      <c r="C39" s="13"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" spans="3:5">
+      <c r="C40" s="13"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="3:5">
+      <c r="C41" s="13"/>
+      <c r="E41" s="13"/>
+    </row>
+    <row r="42" spans="3:5">
+      <c r="C42" s="13"/>
+      <c r="E42" s="13"/>
+    </row>
+    <row r="43" spans="3:5">
+      <c r="C43" s="13"/>
+      <c r="E43" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
@@ -2393,32 +2636,32 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
+  <conditionalFormatting sqref="B30">
     <cfRule type="duplicateValues" dxfId="0" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
+  <conditionalFormatting sqref="B32">
     <cfRule type="duplicateValues" dxfId="0" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
+  <conditionalFormatting sqref="B33">
     <cfRule type="duplicateValues" dxfId="0" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
+  <conditionalFormatting sqref="B35">
     <cfRule type="duplicateValues" dxfId="0" priority="15"/>
     <cfRule type="duplicateValues" dxfId="0" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
+  <conditionalFormatting sqref="B37">
     <cfRule type="duplicateValues" dxfId="0" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A$1:A$1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A33">
+  <conditionalFormatting sqref="A1:A37">
     <cfRule type="duplicateValues" dxfId="0" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 B17:B19 B9:B10 B3 C13 B21:B25 B32 B27">
+  <conditionalFormatting sqref="C1:C7 B17:B19 B9:B10 B3 C13 B21:B29 B31 B36">
     <cfRule type="duplicateValues" dxfId="0" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B6 B8:B10 B12 B16:B19 B21:B30 B32:B1048576">
+  <conditionalFormatting sqref="B2:B6 B8:B10 B12 B16:B19 B21:B34 B36:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2429,266 +2672,337 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="35.4416666666667" customWidth="1"/>
-    <col min="2" max="2" width="29.2166666666667" customWidth="1"/>
+    <col min="1" max="1" width="35.4416666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.2166666666667" style="1" customWidth="1"/>
+    <col min="3" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="12" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:6">
+    <row r="1" ht="15" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" customHeight="1" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" ht="42.75" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" customHeight="1" spans="1:6">
-      <c r="A3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" customHeight="1" spans="1:6">
-      <c r="A4" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" customHeight="1" spans="1:6">
-      <c r="A5" t="s">
+      <c r="B5" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" customHeight="1" spans="1:6">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" customHeight="1" spans="1:6">
-      <c r="A7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" customHeight="1" spans="1:6">
-      <c r="A8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>128</v>
+      <c r="B6" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" customHeight="1" spans="1:6">
-      <c r="A9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" customHeight="1" spans="1:6">
-      <c r="A10" t="s">
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" customHeight="1" spans="1:6">
-      <c r="A11" t="s">
+      <c r="B10" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" customHeight="1" spans="1:6">
-      <c r="A12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" customHeight="1" spans="1:6">
-      <c r="A13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-    </row>
-    <row r="14" customHeight="1" spans="1:6">
-      <c r="A14" t="s">
+      <c r="E11" s="12"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B20" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
-    </row>
-    <row r="15" customHeight="1" spans="1:6">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" customHeight="1" spans="1:6">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" customHeight="1" spans="1:6">
-      <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" customHeight="1" spans="1:6">
-      <c r="A18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" customHeight="1" spans="1:6">
-      <c r="A19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" customHeight="1" spans="1:6">
-      <c r="A20" t="s">
+      <c r="D20" s="13"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B20" t="s">
-        <v>133</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" customHeight="1" spans="1:6">
-      <c r="A21" t="s">
+      <c r="B24" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="10"/>
-    </row>
-    <row r="22" customHeight="1" spans="4:6">
-      <c r="D22" s="8"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" customHeight="1" spans="4:6">
-      <c r="D23" s="8"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" customHeight="1" spans="5:6">
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" customHeight="1" spans="5:6">
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" customHeight="1" spans="5:6">
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" customHeight="1" spans="5:6">
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" customHeight="1" spans="5:6">
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="4:7">
+      <c r="D28" s="13"/>
+      <c r="E28" s="17"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="4:7">
+      <c r="D29" s="13"/>
+      <c r="E29" s="17"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="5:5">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="5:5">
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="5:5">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="4"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">

</xml_diff>